<commit_message>
add azure function startup
</commit_message>
<xml_diff>
--- a/input_data/ipd_nurse/roster_output.xlsx
+++ b/input_data/ipd_nurse/roster_output.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="85">
   <si>
     <t>name_phone</t>
   </si>
@@ -209,30 +209,30 @@
     <t>RN</t>
   </si>
   <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>ME</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>PUB</t>
   </si>
   <si>
     <t>M4</t>
   </si>
   <si>
-    <t>N4</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>PUB</t>
-  </si>
-  <si>
     <t>block</t>
   </si>
   <si>
@@ -248,34 +248,28 @@
     <t>B4</t>
   </si>
   <si>
+    <t>5 (3, 1)</t>
+  </si>
+  <si>
+    <t>5 (3, 2)</t>
+  </si>
+  <si>
+    <t>7 (4, 2)</t>
+  </si>
+  <si>
+    <t>4 (2, 1)</t>
+  </si>
+  <si>
     <t>7 (4, 3)</t>
   </si>
   <si>
-    <t>4 (2, 1)</t>
-  </si>
-  <si>
     <t>4 (2, 2)</t>
   </si>
   <si>
-    <t>6 (3, 2)</t>
-  </si>
-  <si>
-    <t>7 (4, 1)</t>
-  </si>
-  <si>
-    <t>5 (3, 1)</t>
-  </si>
-  <si>
     <t>4 (2, 0)</t>
   </si>
   <si>
-    <t>5 (3, 2)</t>
-  </si>
-  <si>
-    <t>7 (4, 2)</t>
-  </si>
-  <si>
-    <t>5 (3, 0)</t>
+    <t>9 (5, 3)</t>
   </si>
   <si>
     <t>count</t>
@@ -799,85 +793,85 @@
         <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
         <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
         <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" t="s">
         <v>62</v>
       </c>
-      <c r="P2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="AF2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>57</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" t="s">
-        <v>58</v>
-      </c>
-      <c r="V2" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -912,16 +906,16 @@
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O3" t="s">
         <v>61</v>
@@ -930,19 +924,19 @@
         <v>58</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="V3" t="s">
         <v>57</v>
@@ -951,10 +945,10 @@
         <v>58</v>
       </c>
       <c r="X3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="Y3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="Z3" t="s">
         <v>58</v>
@@ -966,25 +960,25 @@
         <v>58</v>
       </c>
       <c r="AC3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF3" t="s">
         <v>62</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AG3" t="s">
         <v>64</v>
       </c>
-      <c r="AE3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>58</v>
-      </c>
       <c r="AH3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AI3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AJ3" t="s">
         <v>58</v>
@@ -1019,82 +1013,82 @@
         <v>59</v>
       </c>
       <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
         <v>57</v>
       </c>
-      <c r="K4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD4" t="s">
         <v>64</v>
       </c>
-      <c r="M4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" t="s">
-        <v>58</v>
-      </c>
-      <c r="S4" t="s">
-        <v>58</v>
-      </c>
-      <c r="T4" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>60</v>
-      </c>
       <c r="AE4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AF4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AG4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="AH4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AI4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ4" t="s">
         <v>59</v>
@@ -1126,88 +1120,88 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
         <v>62</v>
       </c>
       <c r="K5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" t="s">
         <v>57</v>
       </c>
-      <c r="L5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="AC5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" t="s">
         <v>57</v>
       </c>
-      <c r="S5" t="s">
-        <v>58</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="AJ5" t="s">
         <v>60</v>
-      </c>
-      <c r="U5" t="s">
-        <v>60</v>
-      </c>
-      <c r="V5" t="s">
-        <v>59</v>
-      </c>
-      <c r="W5" t="s">
-        <v>58</v>
-      </c>
-      <c r="X5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1236,88 +1230,88 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6" t="s">
         <v>60</v>
       </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="U6" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W6" t="s">
+        <v>61</v>
+      </c>
+      <c r="X6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI6" t="s">
         <v>62</v>
       </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>58</v>
-      </c>
-      <c r="R6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S6" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U6" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" t="s">
-        <v>64</v>
-      </c>
-      <c r="W6" t="s">
-        <v>60</v>
-      </c>
-      <c r="X6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>60</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:36">
@@ -1346,85 +1340,85 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
         <v>58</v>
       </c>
       <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" t="s">
+        <v>58</v>
+      </c>
+      <c r="W7" t="s">
+        <v>58</v>
+      </c>
+      <c r="X7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI7" t="s">
         <v>62</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7" t="s">
-        <v>57</v>
-      </c>
-      <c r="U7" t="s">
-        <v>58</v>
-      </c>
-      <c r="V7" t="s">
-        <v>58</v>
-      </c>
-      <c r="W7" t="s">
-        <v>58</v>
-      </c>
-      <c r="X7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>58</v>
       </c>
       <c r="AJ7" t="s">
         <v>58</v>
@@ -1462,82 +1456,82 @@
         <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
         <v>60</v>
       </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>58</v>
-      </c>
       <c r="O8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q8" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
+        <v>58</v>
+      </c>
+      <c r="W8" t="s">
+        <v>61</v>
+      </c>
+      <c r="X8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE8" t="s">
         <v>62</v>
       </c>
-      <c r="R8" t="s">
+      <c r="AF8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG8" t="s">
         <v>57</v>
       </c>
-      <c r="S8" t="s">
-        <v>58</v>
-      </c>
-      <c r="T8" t="s">
-        <v>62</v>
-      </c>
-      <c r="U8" t="s">
-        <v>58</v>
-      </c>
-      <c r="V8" t="s">
-        <v>58</v>
-      </c>
-      <c r="W8" t="s">
-        <v>58</v>
-      </c>
-      <c r="X8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>59</v>
-      </c>
       <c r="AH8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AI8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AJ8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:36">
@@ -1566,88 +1560,88 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
         <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
         <v>58</v>
       </c>
       <c r="M9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" t="s">
+        <v>58</v>
+      </c>
+      <c r="W9" t="s">
+        <v>63</v>
+      </c>
+      <c r="X9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD9" t="s">
         <v>60</v>
       </c>
-      <c r="N9" t="s">
-        <v>61</v>
-      </c>
-      <c r="O9" t="s">
-        <v>57</v>
-      </c>
-      <c r="P9" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>58</v>
-      </c>
-      <c r="R9" t="s">
-        <v>59</v>
-      </c>
-      <c r="S9" t="s">
-        <v>62</v>
-      </c>
-      <c r="T9" t="s">
-        <v>58</v>
-      </c>
-      <c r="U9" t="s">
-        <v>58</v>
-      </c>
-      <c r="V9" t="s">
-        <v>58</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="AE9" t="s">
         <v>60</v>
       </c>
-      <c r="X9" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC9" t="s">
+      <c r="AF9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>64</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:36">
@@ -1676,76 +1670,76 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
         <v>58</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
         <v>57</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" t="s">
+        <v>59</v>
+      </c>
+      <c r="S10" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" t="s">
+        <v>58</v>
+      </c>
+      <c r="V10" t="s">
+        <v>59</v>
+      </c>
+      <c r="W10" t="s">
+        <v>61</v>
+      </c>
+      <c r="X10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE10" t="s">
         <v>62</v>
       </c>
-      <c r="R10" t="s">
-        <v>57</v>
-      </c>
-      <c r="S10" t="s">
-        <v>57</v>
-      </c>
-      <c r="T10" t="s">
-        <v>61</v>
-      </c>
-      <c r="U10" t="s">
-        <v>58</v>
-      </c>
-      <c r="V10" t="s">
-        <v>61</v>
-      </c>
-      <c r="W10" t="s">
-        <v>58</v>
-      </c>
-      <c r="X10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>58</v>
-      </c>
       <c r="AF10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AG10" t="s">
         <v>58</v>
@@ -1754,7 +1748,7 @@
         <v>58</v>
       </c>
       <c r="AI10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AJ10" t="s">
         <v>59</v>
@@ -1786,20 +1780,20 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" t="s">
         <v>57</v>
       </c>
-      <c r="J11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" t="s">
-        <v>58</v>
-      </c>
-      <c r="M11" t="s">
-        <v>58</v>
-      </c>
       <c r="N11" t="s">
         <v>59</v>
       </c>
@@ -1807,61 +1801,61 @@
         <v>58</v>
       </c>
       <c r="P11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" t="s">
+        <v>58</v>
+      </c>
+      <c r="T11" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" t="s">
-        <v>63</v>
-      </c>
-      <c r="R11" t="s">
-        <v>59</v>
-      </c>
-      <c r="S11" t="s">
-        <v>58</v>
-      </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" t="s">
+        <v>58</v>
+      </c>
+      <c r="W11" t="s">
+        <v>63</v>
+      </c>
+      <c r="X11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE11" t="s">
         <v>62</v>
       </c>
-      <c r="U11" t="s">
-        <v>58</v>
-      </c>
-      <c r="V11" t="s">
-        <v>58</v>
-      </c>
-      <c r="W11" t="s">
-        <v>60</v>
-      </c>
-      <c r="X11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC11" t="s">
+      <c r="AF11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG11" t="s">
         <v>64</v>
       </c>
-      <c r="AD11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>60</v>
-      </c>
       <c r="AH11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AI11" t="s">
         <v>58</v>
@@ -1896,19 +1890,19 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
         <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12" t="s">
         <v>58</v>
@@ -1926,58 +1920,58 @@
         <v>58</v>
       </c>
       <c r="S12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="T12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V12" t="s">
+        <v>58</v>
+      </c>
+      <c r="W12" t="s">
+        <v>61</v>
+      </c>
+      <c r="X12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG12" t="s">
         <v>57</v>
       </c>
-      <c r="U12" t="s">
-        <v>61</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="AH12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>64</v>
-      </c>
-      <c r="W12" t="s">
-        <v>61</v>
-      </c>
-      <c r="X12" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:36">
@@ -2009,19 +2003,19 @@
         <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M13" t="s">
         <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s">
         <v>58</v>
@@ -2030,64 +2024,64 @@
         <v>60</v>
       </c>
       <c r="Q13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="R13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S13" t="s">
         <v>58</v>
       </c>
       <c r="T13" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" t="s">
+        <v>61</v>
+      </c>
+      <c r="V13" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>60</v>
-      </c>
-      <c r="U13" t="s">
-        <v>58</v>
-      </c>
-      <c r="V13" t="s">
-        <v>58</v>
-      </c>
-      <c r="W13" t="s">
-        <v>58</v>
-      </c>
-      <c r="X13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:36">
@@ -2116,19 +2110,19 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
         <v>58</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N14" t="s">
         <v>60</v>
@@ -2140,64 +2134,64 @@
         <v>58</v>
       </c>
       <c r="Q14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S14" t="s">
         <v>57</v>
       </c>
-      <c r="R14" t="s">
-        <v>58</v>
-      </c>
-      <c r="S14" t="s">
-        <v>63</v>
-      </c>
       <c r="T14" t="s">
+        <v>59</v>
+      </c>
+      <c r="U14" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" t="s">
+        <v>58</v>
+      </c>
+      <c r="W14" t="s">
+        <v>58</v>
+      </c>
+      <c r="X14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" t="s">
         <v>60</v>
       </c>
-      <c r="U14" t="s">
-        <v>61</v>
-      </c>
-      <c r="V14" t="s">
-        <v>58</v>
-      </c>
-      <c r="W14" t="s">
-        <v>58</v>
-      </c>
-      <c r="X14" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>58</v>
-      </c>
       <c r="AC14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AD14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG14" t="s">
         <v>64</v>
       </c>
-      <c r="AE14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>57</v>
-      </c>
       <c r="AH14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AI14" t="s">
         <v>61</v>
       </c>
       <c r="AJ14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:36">
@@ -2217,7 +2211,7 @@
         <v>184</v>
       </c>
       <c r="F15">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2226,19 +2220,19 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="L15" t="s">
         <v>58</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N15" t="s">
         <v>58</v>
@@ -2247,10 +2241,10 @@
         <v>63</v>
       </c>
       <c r="P15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="R15" t="s">
         <v>57</v>
@@ -2265,32 +2259,32 @@
         <v>58</v>
       </c>
       <c r="V15" t="s">
+        <v>58</v>
+      </c>
+      <c r="W15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD15" t="s">
         <v>60</v>
       </c>
-      <c r="W15" t="s">
-        <v>60</v>
-      </c>
-      <c r="X15" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>57</v>
-      </c>
       <c r="AE15" t="s">
         <v>61</v>
       </c>
@@ -2298,16 +2292,16 @@
         <v>58</v>
       </c>
       <c r="AG15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AH15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AI15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AJ15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:36">
@@ -2327,7 +2321,7 @@
         <v>184</v>
       </c>
       <c r="F16">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2336,88 +2330,88 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" t="s">
         <v>60</v>
       </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" t="s">
         <v>60</v>
       </c>
-      <c r="M16" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" t="s">
-        <v>58</v>
-      </c>
-      <c r="O16" t="s">
-        <v>60</v>
-      </c>
-      <c r="P16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" t="s">
+        <v>58</v>
+      </c>
+      <c r="U16" t="s">
+        <v>63</v>
+      </c>
+      <c r="V16" t="s">
+        <v>63</v>
+      </c>
+      <c r="W16" t="s">
+        <v>63</v>
+      </c>
+      <c r="X16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF16" t="s">
         <v>62</v>
       </c>
-      <c r="R16" t="s">
-        <v>58</v>
-      </c>
-      <c r="S16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T16" t="s">
-        <v>58</v>
-      </c>
-      <c r="U16" t="s">
-        <v>61</v>
-      </c>
-      <c r="V16" t="s">
+      <c r="AG16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>57</v>
-      </c>
-      <c r="W16" t="s">
-        <v>61</v>
-      </c>
-      <c r="X16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:36">
@@ -2446,28 +2440,28 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L17" t="s">
         <v>61</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="O17" t="s">
         <v>58</v>
       </c>
       <c r="P17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Q17" t="s">
         <v>61</v>
@@ -2476,25 +2470,25 @@
         <v>58</v>
       </c>
       <c r="S17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="U17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="V17" t="s">
         <v>58</v>
       </c>
       <c r="W17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="X17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Y17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z17" t="s">
         <v>58</v>
@@ -2506,25 +2500,25 @@
         <v>58</v>
       </c>
       <c r="AC17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE17" t="s">
         <v>64</v>
       </c>
-      <c r="AD17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>60</v>
-      </c>
       <c r="AF17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AG17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AH17" t="s">
         <v>58</v>
       </c>
       <c r="AI17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AJ17" t="s">
         <v>58</v>
@@ -2556,28 +2550,28 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" t="s">
         <v>57</v>
       </c>
-      <c r="K18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" t="s">
-        <v>61</v>
-      </c>
       <c r="M18" t="s">
         <v>58</v>
       </c>
       <c r="N18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q18" t="s">
         <v>58</v>
@@ -2586,19 +2580,19 @@
         <v>57</v>
       </c>
       <c r="S18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T18" t="s">
         <v>58</v>
       </c>
       <c r="U18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="V18" t="s">
         <v>58</v>
       </c>
       <c r="W18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="X18" t="s">
         <v>58</v>
@@ -2607,10 +2601,10 @@
         <v>61</v>
       </c>
       <c r="Z18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AA18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AB18" t="s">
         <v>58</v>
@@ -2628,16 +2622,16 @@
         <v>61</v>
       </c>
       <c r="AG18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AH18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AJ18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:36">
@@ -2669,7 +2663,7 @@
         <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K19" t="s">
         <v>58</v>
@@ -2678,46 +2672,46 @@
         <v>58</v>
       </c>
       <c r="M19" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" t="s">
         <v>60</v>
       </c>
-      <c r="N19" t="s">
-        <v>58</v>
-      </c>
       <c r="O19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="T19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="U19" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="V19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="X19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Y19" t="s">
         <v>58</v>
       </c>
       <c r="Z19" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA19" t="s">
         <v>61</v>
@@ -2726,16 +2720,16 @@
         <v>61</v>
       </c>
       <c r="AC19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AD19" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AE19" t="s">
         <v>60</v>
       </c>
       <c r="AF19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AG19" t="s">
         <v>58</v>
@@ -2744,7 +2738,7 @@
         <v>58</v>
       </c>
       <c r="AI19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AJ19" t="s">
         <v>58</v>
@@ -2866,79 +2860,79 @@
         <v>71</v>
       </c>
       <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
       <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="Q2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
+        <v>75</v>
+      </c>
+      <c r="U2" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" t="s">
         <v>77</v>
       </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="AA2" t="s">
         <v>75</v>
       </c>
-      <c r="N2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2" t="s">
-        <v>75</v>
-      </c>
-      <c r="V2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>74</v>
-      </c>
       <c r="AB2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AC2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -2949,85 +2943,85 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
         <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="Q3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" t="s">
         <v>71</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>75</v>
       </c>
-      <c r="S3" t="s">
-        <v>72</v>
-      </c>
-      <c r="T3" t="s">
-        <v>72</v>
-      </c>
       <c r="U3" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3" t="s">
         <v>75</v>
       </c>
-      <c r="V3" t="s">
-        <v>71</v>
-      </c>
-      <c r="W3" t="s">
-        <v>72</v>
-      </c>
       <c r="X3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Y3" t="s">
         <v>70</v>
       </c>
       <c r="Z3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AA3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AC3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -3038,85 +3032,85 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="U4" t="s">
         <v>75</v>
-      </c>
-      <c r="O4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" t="s">
-        <v>77</v>
-      </c>
-      <c r="T4" t="s">
-        <v>72</v>
-      </c>
-      <c r="U4" t="s">
-        <v>78</v>
       </c>
       <c r="V4" t="s">
         <v>76</v>
       </c>
       <c r="W4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="X4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Y4" t="s">
         <v>71</v>
       </c>
       <c r="Z4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AA4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AB4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AC4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -3127,85 +3121,85 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
         <v>75</v>
       </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
       <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" t="s">
         <v>71</v>
       </c>
-      <c r="H5" t="s">
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" t="s">
         <v>71</v>
       </c>
-      <c r="I5" t="s">
+      <c r="S5" t="s">
         <v>71</v>
       </c>
-      <c r="J5" t="s">
+      <c r="T5" t="s">
         <v>71</v>
       </c>
-      <c r="K5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="U5" t="s">
         <v>75</v>
       </c>
-      <c r="O5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5" t="s">
-        <v>72</v>
-      </c>
-      <c r="S5" t="s">
-        <v>77</v>
-      </c>
-      <c r="T5" t="s">
-        <v>72</v>
-      </c>
-      <c r="U5" t="s">
-        <v>72</v>
-      </c>
       <c r="V5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="W5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="Y5" t="s">
         <v>71</v>
       </c>
       <c r="Z5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AA5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AC5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3217,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3231,7 +3225,7 @@
         <v>58</v>
       </c>
       <c r="B2">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3239,39 +3233,39 @@
         <v>61</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3279,15 +3273,15 @@
         <v>64</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3308,13 +3302,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3328,10 +3322,10 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3430,10 +3424,10 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3532,10 +3526,10 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3600,10 +3594,10 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3617,10 +3611,10 @@
         <v>9</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3630,7 +3624,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3641,13 +3635,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3655,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>124792</v>
+        <v>253773</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -3681,7 +3675,7 @@
         <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3695,7 +3689,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>61</v>
@@ -3706,16 +3700,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>293806</v>
+        <v>283371</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3729,10 +3723,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
         <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3760,13 +3754,30 @@
         <v>293873</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>293873</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>